<commit_message>
Implemented max drawdown function
</commit_message>
<xml_diff>
--- a/tests/model/dd_model.xlsx
+++ b/tests/model/dd_model.xlsx
@@ -354,11 +354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="331387296"/>
-        <c:axId val="332123248"/>
+        <c:axId val="305411120"/>
+        <c:axId val="305117840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="331387296"/>
+        <c:axId val="305411120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,7 +400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332123248"/>
+        <c:crossAx val="305117840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -408,7 +408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332123248"/>
+        <c:axId val="305117840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +458,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331387296"/>
+        <c:crossAx val="305411120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -649,11 +649,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="341794368"/>
-        <c:axId val="338389392"/>
+        <c:axId val="292583648"/>
+        <c:axId val="307841008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341794368"/>
+        <c:axId val="292583648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338389392"/>
+        <c:crossAx val="307841008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -703,7 +703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="338389392"/>
+        <c:axId val="307841008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,7 +754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341794368"/>
+        <c:crossAx val="292583648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -945,11 +945,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="338344720"/>
-        <c:axId val="332173392"/>
+        <c:axId val="234706080"/>
+        <c:axId val="303311776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="338344720"/>
+        <c:axId val="234706080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -991,7 +991,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332173392"/>
+        <c:crossAx val="303311776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -999,7 +999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332173392"/>
+        <c:axId val="303311776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +1050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338344720"/>
+        <c:crossAx val="234706080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1245,11 +1245,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="332064016"/>
-        <c:axId val="331361280"/>
+        <c:axId val="304066960"/>
+        <c:axId val="303389056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332064016"/>
+        <c:axId val="304066960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,7 +1291,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331361280"/>
+        <c:crossAx val="303389056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1299,7 +1299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="331361280"/>
+        <c:axId val="303389056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1350,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332064016"/>
+        <c:crossAx val="304066960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3967,8 +3967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>